<commit_message>
Updates for TFS 5756. Admin tool access for WPPM50.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C36730
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cms\eCoaching_V2\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cms\eCoaching_V2\Design\DD\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" tabRatio="596"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" tabRatio="596" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="228">
   <si>
     <t>SourceID</t>
   </si>
@@ -218,9 +218,6 @@
     <t>Sr Manager, Customer Service</t>
   </si>
   <si>
-    <t>Sr Analyst, Systems</t>
-  </si>
-  <si>
     <t>WPPM13</t>
   </si>
   <si>
@@ -500,9 +497,6 @@
     <t xml:space="preserve">           ('WTTR50','Manager, Training',5,'Training',1),</t>
   </si>
   <si>
-    <t xml:space="preserve">           ('WPPM13','Sr Analyst, Program',3,'Quality',1) </t>
-  </si>
-  <si>
     <t xml:space="preserve">            INSERT INTO [EC].[AT_Reassign_Status_For_Module]</t>
   </si>
   <si>
@@ -638,9 +632,6 @@
     <t xml:space="preserve">           ('WACS50','Manager, Customer Service',2,'Supervisor',1),</t>
   </si>
   <si>
-    <t xml:space="preserve">           ('WACS60','Sr Manager, Customer Service',1,'CSR',1)</t>
-  </si>
-  <si>
     <t>Replace jobcode WISY13 with WISY14</t>
   </si>
   <si>
@@ -674,15 +665,9 @@
     <t>Sr Specialist, Quality (CS)</t>
   </si>
   <si>
-    <t xml:space="preserve">           ('WACQ13','Sr Specialist, Quality (CS)',103,'WarningAdmin',0,1)</t>
-  </si>
-  <si>
     <t xml:space="preserve">           ('WISY14','Sr Analyst, Systems',103,'WarningAdmin',0,1),</t>
   </si>
   <si>
-    <t xml:space="preserve">      ('WACQ13','Sr Specialist, Quality (CS)',101,'CoachingAdmin',0,1),</t>
-  </si>
-  <si>
     <t>SeniorManager</t>
   </si>
   <si>
@@ -693,6 +678,39 @@
   </si>
   <si>
     <t>Adding rows for SrMgr Dashboard support(Role, Entitlement, Role_Entitlement Link, Role Access Tables</t>
+  </si>
+  <si>
+    <t>Added rows to Role_Access and Module_Access tables for job code WPPM50</t>
+  </si>
+  <si>
+    <t>WPPM50</t>
+  </si>
+  <si>
+    <t>Manager, Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WACS60','Sr Manager, Customer Service',1,'CSR',1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPPM13','Sr Analyst, Program',3,'Quality',1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPPM50','Manager, Program',1,'CSR',1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          ('WPPM50','Manager, Program',2,'Supervisor',1) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WACQ13','Sr Specialist, Quality (CS)',101,'CoachingAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WACQ13','Sr Specialist, Quality (CS)',103,'WarningAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WACS60','Sr Manager, Customer Service',105,'SeniorManager',1,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPPM50','Manager, Program',102,'CoachingUser',1,1)</t>
   </si>
 </sst>
 </file>
@@ -1052,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1069,19 +1087,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1092,13 +1110,13 @@
         <v>42503</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2">
         <v>1709</v>
       </c>
       <c r="E2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1109,13 +1127,13 @@
         <v>42515</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3">
         <v>1709</v>
       </c>
       <c r="E3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1126,13 +1144,13 @@
         <v>42577</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D4">
         <v>3416</v>
       </c>
       <c r="E4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1143,13 +1161,13 @@
         <v>42633</v>
       </c>
       <c r="C5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D5">
         <v>3877</v>
       </c>
       <c r="E5" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1160,13 +1178,30 @@
         <v>42691</v>
       </c>
       <c r="C6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D6">
         <v>3027</v>
       </c>
       <c r="E6" t="s">
-        <v>221</v>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>42797</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7">
+        <v>5756</v>
+      </c>
+      <c r="E7" t="s">
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -1192,16 +1227,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>82</v>
-      </c>
       <c r="F1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1209,13 +1244,13 @@
         <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1223,13 +1258,13 @@
         <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1237,13 +1272,13 @@
         <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1251,13 +1286,13 @@
         <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1265,33 +1300,33 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1316,13 +1351,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="F1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1330,10 +1365,10 @@
         <v>201</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1341,13 +1376,13 @@
         <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1355,10 +1390,10 @@
         <v>203</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1366,10 +1401,10 @@
         <v>204</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1377,10 +1412,10 @@
         <v>205</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1388,10 +1423,10 @@
         <v>206</v>
       </c>
       <c r="B7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1399,10 +1434,10 @@
         <v>207</v>
       </c>
       <c r="B8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F8" t="s">
         <v>194</v>
-      </c>
-      <c r="F8" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1410,15 +1445,15 @@
         <v>208</v>
       </c>
       <c r="B9" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="F9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="F10" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -1443,13 +1478,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1460,7 +1495,7 @@
         <v>201</v>
       </c>
       <c r="F2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1471,7 +1506,7 @@
         <v>202</v>
       </c>
       <c r="F3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1482,7 +1517,7 @@
         <v>203</v>
       </c>
       <c r="F4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1493,7 +1528,7 @@
         <v>204</v>
       </c>
       <c r="F5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1504,7 +1539,7 @@
         <v>206</v>
       </c>
       <c r="F6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1515,7 +1550,7 @@
         <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1526,7 +1561,7 @@
         <v>202</v>
       </c>
       <c r="F8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1537,7 +1572,7 @@
         <v>204</v>
       </c>
       <c r="F9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1548,7 +1583,7 @@
         <v>201</v>
       </c>
       <c r="F10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1559,7 +1594,7 @@
         <v>203</v>
       </c>
       <c r="F11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1570,7 +1605,7 @@
         <v>205</v>
       </c>
       <c r="F12" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1581,7 +1616,7 @@
         <v>207</v>
       </c>
       <c r="F13" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1592,12 +1627,12 @@
         <v>208</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F15" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1625,10 +1660,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>53</v>
@@ -1637,19 +1672,19 @@
         <v>57</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>98</v>
-      </c>
       <c r="M1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1657,7 +1692,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1678,7 +1713,7 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1686,7 +1721,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1707,7 +1742,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1715,7 +1750,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1736,7 +1771,7 @@
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -1765,7 +1800,7 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -1773,7 +1808,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1794,7 +1829,7 @@
         <v>0</v>
       </c>
       <c r="M6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1802,7 +1837,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1823,7 +1858,7 @@
         <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -1831,7 +1866,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1852,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1860,7 +1895,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1881,7 +1916,7 @@
         <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1889,7 +1924,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1910,47 +1945,47 @@
         <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M16" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -1960,11 +1995,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1978,13 +2011,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>108</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>109</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>58</v>
@@ -1993,15 +2026,15 @@
         <v>53</v>
       </c>
       <c r="I1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>215</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2013,15 +2046,15 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>215</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2033,15 +2066,15 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>215</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2053,47 +2086,47 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>215</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>215</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -2113,7 +2146,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2133,55 +2166,55 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
         <v>76</v>
-      </c>
-      <c r="B9" t="s">
-        <v>77</v>
       </c>
       <c r="C9">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" t="s">
         <v>66</v>
-      </c>
-      <c r="B10" t="s">
-        <v>67</v>
       </c>
       <c r="C10">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" t="s">
         <v>64</v>
-      </c>
-      <c r="B11" t="s">
-        <v>65</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -2193,7 +2226,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -2213,7 +2246,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2233,37 +2266,77 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>218</v>
+      </c>
+      <c r="B14" t="s">
+        <v>219</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I14" t="s">
-        <v>154</v>
-      </c>
-    </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>218</v>
+      </c>
+      <c r="B15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
       <c r="I15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I16" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I17" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I19" t="s">
-        <v>157</v>
+        <v>221</v>
+      </c>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="I21" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2288,13 +2361,13 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>12</v>
@@ -2337,7 +2410,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2357,7 +2430,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2371,13 +2444,13 @@
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2397,7 +2470,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2405,7 +2478,7 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -2417,7 +2490,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2425,7 +2498,7 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -2437,7 +2510,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2445,7 +2518,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -2457,52 +2530,52 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -2512,10 +2585,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2530,39 +2603,39 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>53</v>
       </c>
       <c r="K1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C2">
         <v>101</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -2571,21 +2644,21 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C3">
         <v>101</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2594,7 +2667,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -2608,7 +2681,7 @@
         <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2617,7 +2690,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2631,7 +2704,7 @@
         <v>102</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2640,21 +2713,21 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
         <v>76</v>
-      </c>
-      <c r="B6" t="s">
-        <v>77</v>
       </c>
       <c r="C6">
         <v>102</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2663,21 +2736,21 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
         <v>66</v>
-      </c>
-      <c r="B7" t="s">
-        <v>67</v>
       </c>
       <c r="C7">
         <v>102</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2686,21 +2759,21 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
         <v>64</v>
-      </c>
-      <c r="B8" t="s">
-        <v>65</v>
       </c>
       <c r="C8">
         <v>102</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2709,21 +2782,21 @@
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B9" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C9">
         <v>103</v>
       </c>
       <c r="D9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -2732,21 +2805,21 @@
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B10" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C10">
         <v>103</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -2755,7 +2828,7 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2769,46 +2842,74 @@
         <v>105</v>
       </c>
       <c r="D11" t="s">
+        <v>213</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>218</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>219</v>
+      </c>
+      <c r="C12">
+        <v>102</v>
+      </c>
+      <c r="D12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
       <c r="K12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K15" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K16" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K17" t="s">
-        <v>215</v>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K18" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K19" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated fot tfs 6246.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C37002
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" tabRatio="596" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" tabRatio="596"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="233">
   <si>
     <t>SourceID</t>
   </si>
@@ -710,7 +710,22 @@
     <t xml:space="preserve">           ('WACS60','Sr Manager, Customer Service',105,'SeniorManager',1,1),</t>
   </si>
   <si>
-    <t xml:space="preserve">           ('WPPM50','Manager, Program',102,'CoachingUser',1,1)</t>
+    <t>WPSM13</t>
+  </si>
+  <si>
+    <t>Sr Analyst, Functional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPSM13','Sr Analyst, Functional',103,'WarningAdmin',0,1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPSM13','Sr Analyst, Functional',101,'CoachingAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPPM50','Manager, Program',102,'CoachingUser',1,1),</t>
+  </si>
+  <si>
+    <t>Added rows for job code WPSM13 (Mark Hackman)AT_Role_Access tab</t>
   </si>
 </sst>
 </file>
@@ -1070,10 +1085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1202,6 +1217,23 @@
       </c>
       <c r="E7" t="s">
         <v>217</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>42836</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8">
+        <v>6246</v>
+      </c>
+      <c r="E8" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2585,10 +2617,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2878,11 +2910,47 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>227</v>
+      </c>
+      <c r="B13" t="s">
+        <v>228</v>
+      </c>
+      <c r="C13">
+        <v>101</v>
+      </c>
+      <c r="D13" t="s">
+        <v>82</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
       <c r="K13" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>227</v>
+      </c>
+      <c r="B14" t="s">
+        <v>228</v>
+      </c>
+      <c r="C14">
+        <v>103</v>
+      </c>
+      <c r="D14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
       <c r="K14" t="s">
         <v>178</v>
       </c>
@@ -2909,7 +2977,17 @@
     </row>
     <row r="19" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K19" t="s">
-        <v>227</v>
+        <v>231</v>
+      </c>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K20" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K21" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for TFS 5420, 5641 and TFS 5642.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C37251
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" tabRatio="596"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" tabRatio="596" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="310">
   <si>
     <t>SourceID</t>
   </si>
@@ -380,15 +380,6 @@
     <t>('WarningAdmin',1),</t>
   </si>
   <si>
-    <t>('WarningUser',0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          </t>
-  </si>
-  <si>
-    <t>GO</t>
-  </si>
-  <si>
     <t>([RoleDescription],</t>
   </si>
   <si>
@@ -617,18 +608,12 @@
     <t>('ReactivateCoachingLogs'),</t>
   </si>
   <si>
-    <t>('ReactivateWarningLogs')</t>
-  </si>
-  <si>
     <t>(103,205),</t>
   </si>
   <si>
     <t>(101,206),</t>
   </si>
   <si>
-    <t>(103,207)</t>
-  </si>
-  <si>
     <t xml:space="preserve">           ('WACS50','Manager, Customer Service',2,'Supervisor',1),</t>
   </si>
   <si>
@@ -726,6 +711,252 @@
   </si>
   <si>
     <t>Added rows for job code WPSM13 (Mark Hackman)AT_Role_Access tab</t>
+  </si>
+  <si>
+    <t>Added rows to Role, Entitlement, Role Entitlement Link tables to support Reporting</t>
+  </si>
+  <si>
+    <t>Added rows to Role, Entitlement, Role Entitlement Link tables to support Delete functionality in Admin Tool</t>
+  </si>
+  <si>
+    <t>Added rows to Role, Entitlement, Role Entitlement Link tables to support Access control list functionality in Admin Tool</t>
+  </si>
+  <si>
+    <t>ReportCoachingAdmin</t>
+  </si>
+  <si>
+    <t>ReportWarningAdmin</t>
+  </si>
+  <si>
+    <t>ReportCoachingCSRUser</t>
+  </si>
+  <si>
+    <t>ReportWarningCSRUser</t>
+  </si>
+  <si>
+    <t>ReportCoachingSupUser</t>
+  </si>
+  <si>
+    <t>ReportWarningSupUser</t>
+  </si>
+  <si>
+    <t>ReportCoachingQualUser</t>
+  </si>
+  <si>
+    <t>ReportWarningQualUser</t>
+  </si>
+  <si>
+    <t>ReportCoachingLSAUser</t>
+  </si>
+  <si>
+    <t>ReportWarningLSAUser</t>
+  </si>
+  <si>
+    <t>ReportCoachingTrainUser</t>
+  </si>
+  <si>
+    <t>ReportWarningTrainUser</t>
+  </si>
+  <si>
+    <t>SuperUser</t>
+  </si>
+  <si>
+    <t>ACLAdmin</t>
+  </si>
+  <si>
+    <t>Reports</t>
+  </si>
+  <si>
+    <t>Report-RunCoachingSummary</t>
+  </si>
+  <si>
+    <t>Report-RunWarningSummary</t>
+  </si>
+  <si>
+    <t>Report-RunHierarchySummary</t>
+  </si>
+  <si>
+    <t>Report-RunAdminActivitySummary</t>
+  </si>
+  <si>
+    <t>EmployeeLog-SearchForDelete</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>User-eCoachingAccessControlList</t>
+  </si>
+  <si>
+    <t>('Reports'),</t>
+  </si>
+  <si>
+    <t>('Report-RunCoachingSummary'),</t>
+  </si>
+  <si>
+    <t>('Report-RunWarningSummary'),</t>
+  </si>
+  <si>
+    <t>('Report-RunHierarchySummary'),</t>
+  </si>
+  <si>
+    <t>('Report-RunAdminActivitySummary'),</t>
+  </si>
+  <si>
+    <t>('WarningUser',0),</t>
+  </si>
+  <si>
+    <t>('SuperUser',1),</t>
+  </si>
+  <si>
+    <t>('ACLAdmin',1)</t>
+  </si>
+  <si>
+    <t>('SeniorManager'),</t>
+  </si>
+  <si>
+    <t>('ReportWarningAdmin',1),</t>
+  </si>
+  <si>
+    <t>('ReportCoachingCSRUser',0),</t>
+  </si>
+  <si>
+    <t>('ReportWarningCSRUser',0),</t>
+  </si>
+  <si>
+    <t>('ReportCoachingSupUser',0),</t>
+  </si>
+  <si>
+    <t>('ReportWarningSupUser',0),</t>
+  </si>
+  <si>
+    <t>('ReportCoachingQualUser',0),</t>
+  </si>
+  <si>
+    <t>('ReportWarningQualUser',0),</t>
+  </si>
+  <si>
+    <t>('ReportCoachingLSAUser',0),</t>
+  </si>
+  <si>
+    <t>('ReportWarningLSAUser',0),</t>
+  </si>
+  <si>
+    <t>('ReportCoachingTrainUser',0),</t>
+  </si>
+  <si>
+    <t>('ReportCoachingAdmin',1),</t>
+  </si>
+  <si>
+    <t>('ReportWarningTrainUser',0),</t>
+  </si>
+  <si>
+    <t>('ReactivateWarningLogs'),</t>
+  </si>
+  <si>
+    <t>('SeniorManagerDashboard'),</t>
+  </si>
+  <si>
+    <t>('EmployeeLog-SearchForDelete'),</t>
+  </si>
+  <si>
+    <t>('Users'),</t>
+  </si>
+  <si>
+    <t>('User-eCoachingAccessControlList')</t>
+  </si>
+  <si>
+    <t>(103,207),</t>
+  </si>
+  <si>
+    <t>(105,208),</t>
+  </si>
+  <si>
+    <t>(106,209),</t>
+  </si>
+  <si>
+    <t>(106,210),</t>
+  </si>
+  <si>
+    <t>(106,212),</t>
+  </si>
+  <si>
+    <t>(106,213),</t>
+  </si>
+  <si>
+    <t>(107,209),</t>
+  </si>
+  <si>
+    <t>(107,211),</t>
+  </si>
+  <si>
+    <t>(108,209),</t>
+  </si>
+  <si>
+    <t>(108,210),</t>
+  </si>
+  <si>
+    <t>(109,209),</t>
+  </si>
+  <si>
+    <t>(109,211),</t>
+  </si>
+  <si>
+    <t>(110,209),</t>
+  </si>
+  <si>
+    <t>(110,210),</t>
+  </si>
+  <si>
+    <t>(111,209),</t>
+  </si>
+  <si>
+    <t>(111,211),</t>
+  </si>
+  <si>
+    <t>(112,209),</t>
+  </si>
+  <si>
+    <t>(112,210),</t>
+  </si>
+  <si>
+    <t>(113,209),</t>
+  </si>
+  <si>
+    <t>(113,211),</t>
+  </si>
+  <si>
+    <t>(114,209),</t>
+  </si>
+  <si>
+    <t>(114,210),</t>
+  </si>
+  <si>
+    <t>(115,209),</t>
+  </si>
+  <si>
+    <t>(115,211),</t>
+  </si>
+  <si>
+    <t>(116,209),</t>
+  </si>
+  <si>
+    <t>(116,210),</t>
+  </si>
+  <si>
+    <t>(117,209),</t>
+  </si>
+  <si>
+    <t>(117,211),</t>
+  </si>
+  <si>
+    <t>(118,214),</t>
+  </si>
+  <si>
+    <t>(119,215),</t>
+  </si>
+  <si>
+    <t>(119,216)</t>
   </si>
 </sst>
 </file>
@@ -775,12 +1006,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1085,10 +1317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1096,7 +1328,7 @@
     <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="15.88671875" customWidth="1"/>
     <col min="5" max="5" width="144.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1148,7 +1380,7 @@
         <v>1709</v>
       </c>
       <c r="E3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1165,7 +1397,7 @@
         <v>3416</v>
       </c>
       <c r="E4" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1182,7 +1414,7 @@
         <v>3877</v>
       </c>
       <c r="E5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1199,7 +1431,7 @@
         <v>3027</v>
       </c>
       <c r="E6" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1216,7 +1448,7 @@
         <v>5756</v>
       </c>
       <c r="E7" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1233,7 +1465,40 @@
         <v>6246</v>
       </c>
       <c r="E8" t="s">
-        <v>232</v>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>42856</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9">
+        <v>5420</v>
+      </c>
+      <c r="E9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>5641</v>
+      </c>
+      <c r="E10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>5642</v>
+      </c>
+      <c r="E11" t="s">
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -1244,16 +1509,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" customWidth="1"/>
     <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1282,7 +1545,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1332,7 +1595,7 @@
         <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1342,23 +1605,214 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
       <c r="F7" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>232</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
       <c r="F8" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>233</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>234</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s">
+        <v>236</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>112</v>
+      </c>
+      <c r="B13" t="s">
+        <v>237</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>113</v>
+      </c>
+      <c r="B14" t="s">
+        <v>238</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>114</v>
+      </c>
+      <c r="B15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="F15" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>115</v>
+      </c>
+      <c r="B16" t="s">
+        <v>240</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>116</v>
+      </c>
+      <c r="B17" t="s">
+        <v>241</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>117</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F10" t="s">
+      <c r="B18" t="s">
+        <v>242</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
         <v>118</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F11" t="s">
+      <c r="B19" t="s">
+        <v>243</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>119</v>
+      </c>
+      <c r="B20" t="s">
+        <v>244</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>
@@ -1368,11 +1822,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1389,7 +1841,7 @@
         <v>87</v>
       </c>
       <c r="F1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1400,7 +1852,7 @@
         <v>88</v>
       </c>
       <c r="F2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -1414,7 +1866,7 @@
         <v>113</v>
       </c>
       <c r="H3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1425,7 +1877,7 @@
         <v>90</v>
       </c>
       <c r="F4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -1436,7 +1888,7 @@
         <v>91</v>
       </c>
       <c r="F5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -1447,7 +1899,7 @@
         <v>92</v>
       </c>
       <c r="F6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -1455,10 +1907,10 @@
         <v>206</v>
       </c>
       <c r="B7" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1466,10 +1918,10 @@
         <v>207</v>
       </c>
       <c r="B8" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F8" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -1477,15 +1929,108 @@
         <v>208</v>
       </c>
       <c r="B9" t="s">
+        <v>209</v>
+      </c>
+      <c r="F9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>209</v>
+      </c>
+      <c r="B10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>210</v>
+      </c>
+      <c r="B11" t="s">
+        <v>246</v>
+      </c>
+      <c r="F11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>211</v>
+      </c>
+      <c r="B12" t="s">
+        <v>247</v>
+      </c>
+      <c r="F12" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>212</v>
+      </c>
+      <c r="B13" t="s">
+        <v>248</v>
+      </c>
+      <c r="F13" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>213</v>
+      </c>
+      <c r="B14" t="s">
+        <v>249</v>
+      </c>
+      <c r="F14" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
         <v>214</v>
       </c>
-      <c r="F9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F10" t="s">
-        <v>196</v>
+      <c r="B15" t="s">
+        <v>250</v>
+      </c>
+      <c r="F15" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>215</v>
+      </c>
+      <c r="B16" t="s">
+        <v>251</v>
+      </c>
+      <c r="F16" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>216</v>
+      </c>
+      <c r="B17" t="s">
+        <v>252</v>
+      </c>
+      <c r="F17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -1495,10 +2040,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1516,7 +2061,7 @@
         <v>86</v>
       </c>
       <c r="F1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1527,7 +2072,7 @@
         <v>201</v>
       </c>
       <c r="F2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -1549,7 +2094,7 @@
         <v>203</v>
       </c>
       <c r="F4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -1560,7 +2105,7 @@
         <v>204</v>
       </c>
       <c r="F5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -1571,7 +2116,7 @@
         <v>206</v>
       </c>
       <c r="F6" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -1582,7 +2127,7 @@
         <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -1593,7 +2138,7 @@
         <v>202</v>
       </c>
       <c r="F8" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1604,7 +2149,7 @@
         <v>204</v>
       </c>
       <c r="F9" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1615,7 +2160,7 @@
         <v>201</v>
       </c>
       <c r="F10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1626,7 +2171,7 @@
         <v>203</v>
       </c>
       <c r="F11" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1637,7 +2182,7 @@
         <v>205</v>
       </c>
       <c r="F12" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1648,7 +2193,7 @@
         <v>207</v>
       </c>
       <c r="F13" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1659,12 +2204,336 @@
         <v>208</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>106</v>
+      </c>
+      <c r="B15">
+        <v>209</v>
+      </c>
       <c r="F15" s="4" t="s">
-        <v>199</v>
+        <v>279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>106</v>
+      </c>
+      <c r="B16">
+        <v>210</v>
+      </c>
+      <c r="F16" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>106</v>
+      </c>
+      <c r="B17">
+        <v>212</v>
+      </c>
+      <c r="F17" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>106</v>
+      </c>
+      <c r="B18">
+        <v>213</v>
+      </c>
+      <c r="F18" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>107</v>
+      </c>
+      <c r="B19">
+        <v>209</v>
+      </c>
+      <c r="F19" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>107</v>
+      </c>
+      <c r="B20">
+        <v>211</v>
+      </c>
+      <c r="F20" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>108</v>
+      </c>
+      <c r="B21">
+        <v>209</v>
+      </c>
+      <c r="F21" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>108</v>
+      </c>
+      <c r="B22">
+        <v>210</v>
+      </c>
+      <c r="F22" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>109</v>
+      </c>
+      <c r="B23">
+        <v>209</v>
+      </c>
+      <c r="F23" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>109</v>
+      </c>
+      <c r="B24">
+        <v>211</v>
+      </c>
+      <c r="F24" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>110</v>
+      </c>
+      <c r="B25">
+        <v>209</v>
+      </c>
+      <c r="F25" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>110</v>
+      </c>
+      <c r="B26">
+        <v>210</v>
+      </c>
+      <c r="F26" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>111</v>
+      </c>
+      <c r="B27">
+        <v>209</v>
+      </c>
+      <c r="F27" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>111</v>
+      </c>
+      <c r="B28">
+        <v>211</v>
+      </c>
+      <c r="F28" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>112</v>
+      </c>
+      <c r="B29">
+        <v>209</v>
+      </c>
+      <c r="F29" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>112</v>
+      </c>
+      <c r="B30">
+        <v>210</v>
+      </c>
+      <c r="F30" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>113</v>
+      </c>
+      <c r="B31">
+        <v>209</v>
+      </c>
+      <c r="F31" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>113</v>
+      </c>
+      <c r="B32">
+        <v>211</v>
+      </c>
+      <c r="F32" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>114</v>
+      </c>
+      <c r="B33">
+        <v>209</v>
+      </c>
+      <c r="F33" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>114</v>
+      </c>
+      <c r="B34">
+        <v>210</v>
+      </c>
+      <c r="F34" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>115</v>
+      </c>
+      <c r="B35">
+        <v>209</v>
+      </c>
+      <c r="F35" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>115</v>
+      </c>
+      <c r="B36">
+        <v>211</v>
+      </c>
+      <c r="F36" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>116</v>
+      </c>
+      <c r="B37">
+        <v>209</v>
+      </c>
+      <c r="F37" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>116</v>
+      </c>
+      <c r="B38">
+        <v>210</v>
+      </c>
+      <c r="F38" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>117</v>
+      </c>
+      <c r="B39">
+        <v>209</v>
+      </c>
+      <c r="F39" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>117</v>
+      </c>
+      <c r="B40">
+        <v>211</v>
+      </c>
+      <c r="F40" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>118</v>
+      </c>
+      <c r="B41">
+        <v>214</v>
+      </c>
+      <c r="F41" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>119</v>
+      </c>
+      <c r="B42">
+        <v>215</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>119</v>
+      </c>
+      <c r="B43">
+        <v>216</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F45" s="5" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -1716,7 +2585,7 @@
         <v>97</v>
       </c>
       <c r="M1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -1745,7 +2614,7 @@
         <v>0</v>
       </c>
       <c r="M2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -1774,7 +2643,7 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -1803,7 +2672,7 @@
         <v>0</v>
       </c>
       <c r="M4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -1832,7 +2701,7 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -1861,7 +2730,7 @@
         <v>0</v>
       </c>
       <c r="M6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -1890,7 +2759,7 @@
         <v>0</v>
       </c>
       <c r="M7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -1919,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -1948,7 +2817,7 @@
         <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -1977,47 +2846,47 @@
         <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M11" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M12" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M14" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M15" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="M16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M17" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="13:13" x14ac:dyDescent="0.3">
       <c r="M18" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2058,15 +2927,15 @@
         <v>53</v>
       </c>
       <c r="I1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2078,15 +2947,15 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2098,15 +2967,15 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2118,15 +2987,15 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B5" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2138,15 +3007,15 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -2158,7 +3027,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -2178,7 +3047,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -2198,7 +3067,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -2218,7 +3087,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -2238,7 +3107,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -2258,7 +3127,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -2278,7 +3147,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2298,15 +3167,15 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B14" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2318,15 +3187,15 @@
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B15" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -2338,37 +3207,37 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="I16" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I17" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I18" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I19" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I20" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
     </row>
     <row r="21" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I21" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2442,7 +3311,7 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -2462,7 +3331,7 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2482,7 +3351,7 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2502,7 +3371,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2522,7 +3391,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2542,7 +3411,7 @@
         <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2562,52 +3431,52 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J11" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J12" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J14" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J15" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="J16" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J17" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="18" spans="10:10" x14ac:dyDescent="0.3">
       <c r="J18" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -2647,21 +3516,21 @@
         <v>80</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>53</v>
       </c>
       <c r="K1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C2">
         <v>101</v>
@@ -2676,15 +3545,15 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C3">
         <v>101</v>
@@ -2699,7 +3568,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -2722,7 +3591,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2745,7 +3614,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -2768,7 +3637,7 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -2791,7 +3660,7 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -2814,15 +3683,15 @@
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B9" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C9">
         <v>103</v>
@@ -2837,15 +3706,15 @@
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B10" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="C10">
         <v>103</v>
@@ -2860,7 +3729,7 @@
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2874,7 +3743,7 @@
         <v>105</v>
       </c>
       <c r="D11" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -2883,15 +3752,15 @@
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B12" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C12">
         <v>102</v>
@@ -2906,15 +3775,15 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B13" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C13">
         <v>101</v>
@@ -2929,15 +3798,15 @@
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B14" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C14">
         <v>103</v>
@@ -2952,42 +3821,42 @@
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K15" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K16" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K17" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K18" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K19" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K20" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K21" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for TFS 6591 to add Brian Coughlins job code to AT_Role_Access table.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C37555
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" tabRatio="596" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" tabRatio="596" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="337">
   <si>
     <t>SourceID</t>
   </si>
@@ -701,9 +701,6 @@
     <t>Sr Analyst, Functional</t>
   </si>
   <si>
-    <t xml:space="preserve">           ('WPSM13','Sr Analyst, Functional',103,'WarningAdmin',0,1)</t>
-  </si>
-  <si>
     <t xml:space="preserve">           ('WPSM13','Sr Analyst, Functional',101,'CoachingAdmin',0,1),</t>
   </si>
   <si>
@@ -957,6 +954,90 @@
   </si>
   <si>
     <t>(119,216)</t>
+  </si>
+  <si>
+    <t>Added rows for job code WSTE14 (Brian Coughlin)AT_Role_Access tab</t>
+  </si>
+  <si>
+    <t>WISO12</t>
+  </si>
+  <si>
+    <t>Engineer, Software</t>
+  </si>
+  <si>
+    <t>WISO13</t>
+  </si>
+  <si>
+    <t>Sr Engineer, Software</t>
+  </si>
+  <si>
+    <t>WSTE12</t>
+  </si>
+  <si>
+    <t>Engineer, Test</t>
+  </si>
+  <si>
+    <t>WSTE13</t>
+  </si>
+  <si>
+    <t>Sr Engineer, Test</t>
+  </si>
+  <si>
+    <t>WSTE14</t>
+  </si>
+  <si>
+    <t>Principal Engineer, Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPSM13','Sr Analyst, Functional',103,'WarningAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WSTE14','Principal Engineer, Test',106,'ReportCoachingAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          ('WISO12','Engineer, Software',106,'ReportCoachingAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WISO12','Engineer, Software',107,'ReportWarningAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WISO13','Sr Engineer, Software',106,'ReportCoachingAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WISO13','Sr Engineer, Software',107,'ReportWarningAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WSTE12','Engineer, Test',106,'ReportCoachingAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WSTE12','Engineer, Test',107,'ReportWarningAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WSTE13','Sr Engineer, Test',106,'ReportCoachingAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WSTE13','Sr Engineer, Test',107,'ReportWarningAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WISY14','Principal Analyst, Systems',106,'ReportCoachingAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WISY14','Principal Analyst, Systems',107,'ReportWarningAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WACQ13','Sr Specialist, Quality (CS)',106,'ReportCoachingAdmin',0,1),  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WACQ13','Sr Specialist, Quality (CS)',107,'ReportWarningAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPSM13','Sr Analyst, Functional',106,'ReportCoachingAdmin',0,1),  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPSM13','Sr Analyst, Functional',107,'ReportWarningAdmin',0,1)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WSTE14','Principal Engineer, Test',107,'ReportWarningAdmin',0,1),</t>
   </si>
 </sst>
 </file>
@@ -1317,11 +1398,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1465,7 +1544,7 @@
         <v>6246</v>
       </c>
       <c r="E8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1482,7 +1561,7 @@
         <v>5420</v>
       </c>
       <c r="E9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1490,7 +1569,7 @@
         <v>5641</v>
       </c>
       <c r="E10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1498,7 +1577,24 @@
         <v>5642</v>
       </c>
       <c r="E11" t="s">
-        <v>230</v>
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="1">
+        <v>42877</v>
+      </c>
+      <c r="C12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12">
+        <v>6591</v>
+      </c>
+      <c r="E12" t="s">
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -1609,7 +1705,7 @@
         <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1623,13 +1719,13 @@
         <v>107</v>
       </c>
       <c r="B8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1637,13 +1733,13 @@
         <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -1651,13 +1747,13 @@
         <v>109</v>
       </c>
       <c r="B10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -1665,13 +1761,13 @@
         <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1679,13 +1775,13 @@
         <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1693,13 +1789,13 @@
         <v>112</v>
       </c>
       <c r="B13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1707,13 +1803,13 @@
         <v>113</v>
       </c>
       <c r="B14" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1721,13 +1817,13 @@
         <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1735,13 +1831,13 @@
         <v>115</v>
       </c>
       <c r="B16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1749,13 +1845,13 @@
         <v>116</v>
       </c>
       <c r="B17" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1763,13 +1859,13 @@
         <v>117</v>
       </c>
       <c r="B18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1777,13 +1873,13 @@
         <v>118</v>
       </c>
       <c r="B19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1791,28 +1887,28 @@
         <v>119</v>
       </c>
       <c r="B20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F21" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F23" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -1940,10 +2036,10 @@
         <v>209</v>
       </c>
       <c r="B10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -1951,10 +2047,10 @@
         <v>210</v>
       </c>
       <c r="B11" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -1962,10 +2058,10 @@
         <v>211</v>
       </c>
       <c r="B12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F12" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -1973,10 +2069,10 @@
         <v>212</v>
       </c>
       <c r="B13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F13" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -1984,10 +2080,10 @@
         <v>213</v>
       </c>
       <c r="B14" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -1995,10 +2091,10 @@
         <v>214</v>
       </c>
       <c r="B15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -2006,10 +2102,10 @@
         <v>215</v>
       </c>
       <c r="B16" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F16" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2017,20 +2113,20 @@
         <v>216</v>
       </c>
       <c r="B17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="F17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F18" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F19" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -2042,7 +2138,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
@@ -2215,7 +2311,7 @@
         <v>209</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -2226,7 +2322,7 @@
         <v>210</v>
       </c>
       <c r="F16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -2237,7 +2333,7 @@
         <v>212</v>
       </c>
       <c r="F17" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -2248,7 +2344,7 @@
         <v>213</v>
       </c>
       <c r="F18" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -2259,7 +2355,7 @@
         <v>209</v>
       </c>
       <c r="F19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -2270,7 +2366,7 @@
         <v>211</v>
       </c>
       <c r="F20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -2281,7 +2377,7 @@
         <v>209</v>
       </c>
       <c r="F21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -2292,7 +2388,7 @@
         <v>210</v>
       </c>
       <c r="F22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -2303,7 +2399,7 @@
         <v>209</v>
       </c>
       <c r="F23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -2314,7 +2410,7 @@
         <v>211</v>
       </c>
       <c r="F24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -2325,7 +2421,7 @@
         <v>209</v>
       </c>
       <c r="F25" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -2336,7 +2432,7 @@
         <v>210</v>
       </c>
       <c r="F26" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -2347,7 +2443,7 @@
         <v>209</v>
       </c>
       <c r="F27" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -2358,7 +2454,7 @@
         <v>211</v>
       </c>
       <c r="F28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -2369,7 +2465,7 @@
         <v>209</v>
       </c>
       <c r="F29" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -2380,7 +2476,7 @@
         <v>210</v>
       </c>
       <c r="F30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -2391,7 +2487,7 @@
         <v>209</v>
       </c>
       <c r="F31" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -2402,7 +2498,7 @@
         <v>211</v>
       </c>
       <c r="F32" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -2413,7 +2509,7 @@
         <v>209</v>
       </c>
       <c r="F33" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
@@ -2424,7 +2520,7 @@
         <v>210</v>
       </c>
       <c r="F34" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -2435,7 +2531,7 @@
         <v>209</v>
       </c>
       <c r="F35" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
@@ -2446,7 +2542,7 @@
         <v>211</v>
       </c>
       <c r="F36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -2457,7 +2553,7 @@
         <v>209</v>
       </c>
       <c r="F37" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2468,7 +2564,7 @@
         <v>210</v>
       </c>
       <c r="F38" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -2479,7 +2575,7 @@
         <v>209</v>
       </c>
       <c r="F39" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
@@ -2490,7 +2586,7 @@
         <v>211</v>
       </c>
       <c r="F40" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2501,7 +2597,7 @@
         <v>214</v>
       </c>
       <c r="F41" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -2512,7 +2608,7 @@
         <v>215</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
@@ -2523,17 +2619,17 @@
         <v>216</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F44" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F45" s="5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>
@@ -3486,10 +3582,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3527,10 +3623,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C2">
         <v>101</v>
@@ -3556,10 +3652,10 @@
         <v>206</v>
       </c>
       <c r="C3">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -3573,19 +3669,19 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>205</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>206</v>
       </c>
       <c r="C4">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>230</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -3596,19 +3692,19 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>205</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>206</v>
       </c>
       <c r="C5">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>231</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -3619,10 +3715,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C6">
         <v>102</v>
@@ -3642,10 +3738,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C7">
         <v>102</v>
@@ -3665,16 +3761,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C8">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>208</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -3688,19 +3784,19 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
-        <v>210</v>
+        <v>76</v>
       </c>
       <c r="C9">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -3711,16 +3807,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>205</v>
+        <v>310</v>
       </c>
       <c r="B10" t="s">
-        <v>206</v>
+        <v>311</v>
       </c>
       <c r="C10">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>230</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -3734,19 +3830,19 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>310</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>311</v>
       </c>
       <c r="C11">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D11" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="E11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -3757,19 +3853,19 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>213</v>
+        <v>312</v>
       </c>
       <c r="B12" t="s">
-        <v>214</v>
+        <v>313</v>
       </c>
       <c r="C12">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>230</v>
       </c>
       <c r="E12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -3780,16 +3876,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>222</v>
+        <v>312</v>
       </c>
       <c r="B13" t="s">
-        <v>223</v>
+        <v>313</v>
       </c>
       <c r="C13">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>231</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -3803,16 +3899,16 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>222</v>
+        <v>197</v>
       </c>
       <c r="B14" t="s">
-        <v>223</v>
+        <v>210</v>
       </c>
       <c r="C14">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -3825,38 +3921,406 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>197</v>
+      </c>
+      <c r="B15" t="s">
+        <v>210</v>
+      </c>
+      <c r="C15">
+        <v>106</v>
+      </c>
+      <c r="D15" t="s">
+        <v>230</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
       <c r="K15" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" t="s">
+        <v>210</v>
+      </c>
+      <c r="C16">
+        <v>107</v>
+      </c>
+      <c r="D16" t="s">
+        <v>231</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
       <c r="K16" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>197</v>
+      </c>
+      <c r="B17" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17">
+        <v>103</v>
+      </c>
+      <c r="D17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
       <c r="K17" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18">
+        <v>102</v>
+      </c>
+      <c r="D18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
       <c r="K18" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B19" t="s">
+        <v>214</v>
+      </c>
+      <c r="C19">
+        <v>102</v>
+      </c>
+      <c r="D19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
       <c r="K19" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.3">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>222</v>
+      </c>
+      <c r="B20" t="s">
+        <v>223</v>
+      </c>
+      <c r="C20">
+        <v>101</v>
+      </c>
+      <c r="D20" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
       <c r="K20" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="21" spans="11:11" x14ac:dyDescent="0.3">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>222</v>
+      </c>
+      <c r="B21" t="s">
+        <v>223</v>
+      </c>
+      <c r="C21">
+        <v>103</v>
+      </c>
+      <c r="D21" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
       <c r="K21" t="s">
-        <v>224</v>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>222</v>
+      </c>
+      <c r="B22" t="s">
+        <v>223</v>
+      </c>
+      <c r="C22">
+        <v>106</v>
+      </c>
+      <c r="D22" t="s">
+        <v>230</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="K22" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>222</v>
+      </c>
+      <c r="B23" t="s">
+        <v>223</v>
+      </c>
+      <c r="C23">
+        <v>107</v>
+      </c>
+      <c r="D23" t="s">
+        <v>231</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="K23" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>314</v>
+      </c>
+      <c r="B24" t="s">
+        <v>315</v>
+      </c>
+      <c r="C24">
+        <v>106</v>
+      </c>
+      <c r="D24" t="s">
+        <v>230</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="K24" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>314</v>
+      </c>
+      <c r="B25" t="s">
+        <v>315</v>
+      </c>
+      <c r="C25">
+        <v>107</v>
+      </c>
+      <c r="D25" t="s">
+        <v>231</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="K25" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>316</v>
+      </c>
+      <c r="B26" t="s">
+        <v>317</v>
+      </c>
+      <c r="C26">
+        <v>106</v>
+      </c>
+      <c r="D26" t="s">
+        <v>230</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="K26" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>316</v>
+      </c>
+      <c r="B27" t="s">
+        <v>317</v>
+      </c>
+      <c r="C27">
+        <v>107</v>
+      </c>
+      <c r="D27" t="s">
+        <v>231</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="K27" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>318</v>
+      </c>
+      <c r="B28" t="s">
+        <v>319</v>
+      </c>
+      <c r="C28">
+        <v>106</v>
+      </c>
+      <c r="D28" t="s">
+        <v>230</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>318</v>
+      </c>
+      <c r="B29" t="s">
+        <v>319</v>
+      </c>
+      <c r="C29">
+        <v>107</v>
+      </c>
+      <c r="D29" t="s">
+        <v>231</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="K29" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30">
+        <v>102</v>
+      </c>
+      <c r="D30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="K30" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K31" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K32" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K33" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="34" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K34" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K35" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K36" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="37" spans="11:11" x14ac:dyDescent="0.3">
+      <c r="K37" t="s">
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for TFS 8363. Admin tool access for new Program team members.
git-tfs-id: [https://tfs.omnicloud.local/tfs/cco%20program/]$/eCoaching_V2;C38681
</commit_message>
<xml_diff>
--- a/Design/DD/DB/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
+++ b/Design/DD/DB/CCO_eCoaching_AT_Dimension_Table_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" tabRatio="596" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="22992" windowHeight="12840" tabRatio="596"/>
   </bookViews>
   <sheets>
     <sheet name="Revision_History" sheetId="14" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="344">
   <si>
     <t>SourceID</t>
   </si>
@@ -1034,10 +1034,31 @@
     <t xml:space="preserve">           ('WPSM13','Sr Analyst, Functional',106,'ReportCoachingAdmin',0,1),  </t>
   </si>
   <si>
-    <t xml:space="preserve">           ('WPSM13','Sr Analyst, Functional',107,'ReportWarningAdmin',0,1)   </t>
-  </si>
-  <si>
     <t xml:space="preserve">           ('WSTE14','Principal Engineer, Test',107,'ReportWarningAdmin',0,1),</t>
+  </si>
+  <si>
+    <t>WPPM11</t>
+  </si>
+  <si>
+    <t>Associate Analyst, Program</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPSM13','Sr Analyst, Functional',107,'ReportWarningAdmin',0,1) ,  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPPM11','Associate Analyst, Program',101,'CoachingAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPPM11','Associate Analyst, Program',103,'WarningAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPPM11','Associate Analyst, Program',106,'ReportCoachingAdmin',0,1),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           ('WPPM11','Associate Analyst, Program',107,'ReportWarningAdmin',0,1)</t>
+  </si>
+  <si>
+    <t>Added rows for job code WPPM11 (New program staff ) in AT_Role_Access tab</t>
   </si>
 </sst>
 </file>
@@ -1398,9 +1419,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1595,6 +1616,23 @@
       </c>
       <c r="E12" t="s">
         <v>309</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1">
+        <v>43000</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13">
+        <v>8363</v>
+      </c>
+      <c r="E13" t="s">
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -3582,11 +3620,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4124,7 +4160,7 @@
         <v>1</v>
       </c>
       <c r="K23" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -4289,38 +4325,130 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>336</v>
+      </c>
+      <c r="B31" t="s">
+        <v>337</v>
+      </c>
+      <c r="C31">
+        <v>101</v>
+      </c>
+      <c r="D31" t="s">
+        <v>82</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
       <c r="K31" t="s">
         <v>329</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>336</v>
+      </c>
+      <c r="B32" t="s">
+        <v>337</v>
+      </c>
+      <c r="C32">
+        <v>103</v>
+      </c>
+      <c r="D32" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
       <c r="K32" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>336</v>
+      </c>
+      <c r="B33" t="s">
+        <v>337</v>
+      </c>
+      <c r="C33">
+        <v>106</v>
+      </c>
+      <c r="D33" t="s">
+        <v>230</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
       <c r="K33" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="34" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>336</v>
+      </c>
+      <c r="B34" t="s">
+        <v>337</v>
+      </c>
+      <c r="C34">
+        <v>107</v>
+      </c>
+      <c r="D34" t="s">
+        <v>231</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
       <c r="K34" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="35" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K35" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="36" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K36" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="37" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="K37" t="s">
-        <v>335</v>
+        <v>338</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K38" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K39" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K40" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K41" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>